<commit_message>
fix format number harga input with js
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_inventaris_ruangan - Copy.xlsx
+++ b/public/templates/template_aset_inventaris_ruangan - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12B1601-7F77-495E-A022-12D443F4ACD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD9A59F-E9CF-4491-9EFA-59C4D2153803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{EA767793-6A0C-4171-AE55-10E9968E0A80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>id_status_aset</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Bufet</t>
+  </si>
+  <si>
+    <t>Komputer</t>
+  </si>
+  <si>
+    <t>Laptop Acer Aspire 5</t>
+  </si>
+  <si>
+    <t>27/12/2023</t>
+  </si>
+  <si>
+    <t>Metal</t>
   </si>
 </sst>
 </file>
@@ -452,17 +464,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD9F2F5-63C9-41E4-A43D-AA50754BEB26}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -577,6 +589,41 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>2017</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>8500000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>